<commit_message>
exceli tagasi kirjutamine, pie chart, trend chart, kulud, tulud ja kulude/tulude summad erineval exceli sheetil
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="40">
   <si>
     <t>Kategooria</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>EUR</t>
+  </si>
+  <si>
+    <t>Kulude summa</t>
+  </si>
+  <si>
+    <t>Tulude summa</t>
   </si>
 </sst>
 </file>
@@ -209,16 +215,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>11</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>114313</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -235,8 +241,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6705600" y="190500"/>
-          <a:ext cx="5486411" cy="6400813"/>
+          <a:off x="4267200" y="190500"/>
+          <a:ext cx="5486411" cy="5486411"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -247,16 +253,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>15</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>38107</xdr:rowOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>114313</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -273,8 +279,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6705600" y="4000500"/>
-          <a:ext cx="7315215" cy="3657607"/>
+          <a:off x="4267200" y="6477000"/>
+          <a:ext cx="7315215" cy="6400813"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1605,108 +1611,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:8">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B4">
         <v>56</v>
       </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>550</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B5">
         <v>1.49</v>
       </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>4.99</v>
       </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
         <v>294.78</v>
       </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>240.88</v>
       </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>21.26</v>
       </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Visualiseeri ja tkinter teised lehed
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -261,8 +261,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>15</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>114313</xdr:rowOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>38112</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -280,7 +280,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4267200" y="6477000"/>
-          <a:ext cx="7315215" cy="6400813"/>
+          <a:ext cx="7315215" cy="5943612"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1611,16 +1611,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="2" spans="1:8">
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
       <c r="F2" t="s">
         <v>39</v>
       </c>

</xml_diff>